<commit_message>
checkpoint g13; feito t13.2
</commit_message>
<xml_diff>
--- a/Data/t13.2.xlsx
+++ b/Data/t13.2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01/10/2012</t>
+          <t>31/10/2012</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -496,7 +496,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01/10/2012</t>
+          <t>31/10/2012</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -519,7 +519,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01/10/2012</t>
+          <t>31/10/2012</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -542,7 +542,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01/10/2012</t>
+          <t>31/10/2012</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,7 +565,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01/10/2012</t>
+          <t>31/10/2012</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -588,7 +588,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>01/10/2012</t>
+          <t>31/10/2012</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -611,7 +611,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>01/10/2012</t>
+          <t>31/10/2012</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -634,7 +634,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>01/10/2012</t>
+          <t>31/10/2012</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -657,7 +657,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>01/10/2013</t>
+          <t>31/10/2013</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -680,7 +680,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>01/10/2013</t>
+          <t>31/10/2013</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -703,7 +703,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>01/10/2013</t>
+          <t>31/10/2013</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -726,7 +726,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>01/10/2013</t>
+          <t>31/10/2013</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -749,7 +749,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>01/10/2013</t>
+          <t>31/10/2013</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -772,7 +772,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>01/10/2013</t>
+          <t>31/10/2013</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -795,7 +795,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>01/10/2013</t>
+          <t>31/10/2013</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -818,7 +818,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>01/10/2013</t>
+          <t>31/10/2013</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>01/10/2014</t>
+          <t>31/10/2014</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -864,7 +864,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>01/10/2014</t>
+          <t>31/10/2014</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -887,7 +887,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>01/10/2014</t>
+          <t>31/10/2014</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -910,7 +910,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>01/10/2014</t>
+          <t>31/10/2014</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -933,7 +933,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>01/10/2014</t>
+          <t>31/10/2014</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -956,7 +956,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>01/10/2014</t>
+          <t>31/10/2014</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -979,7 +979,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>01/10/2014</t>
+          <t>31/10/2014</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>01/10/2014</t>
+          <t>31/10/2014</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1025,7 +1025,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>01/10/2015</t>
+          <t>31/10/2015</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>01/10/2015</t>
+          <t>31/10/2015</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>01/10/2015</t>
+          <t>31/10/2015</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>01/10/2015</t>
+          <t>31/10/2015</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>01/10/2015</t>
+          <t>31/10/2015</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>01/10/2015</t>
+          <t>31/10/2015</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>01/10/2015</t>
+          <t>31/10/2015</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>01/10/2015</t>
+          <t>31/10/2015</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>01/10/2016</t>
+          <t>31/10/2016</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1232,7 +1232,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>01/10/2016</t>
+          <t>31/10/2016</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>01/10/2016</t>
+          <t>31/10/2016</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>01/10/2016</t>
+          <t>31/10/2016</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>01/10/2016</t>
+          <t>31/10/2016</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>01/10/2016</t>
+          <t>31/10/2016</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>01/10/2016</t>
+          <t>31/10/2016</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>01/10/2016</t>
+          <t>31/10/2016</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>01/10/2017</t>
+          <t>31/10/2017</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>01/10/2017</t>
+          <t>31/10/2017</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>01/10/2017</t>
+          <t>31/10/2017</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1462,7 +1462,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>01/10/2017</t>
+          <t>31/10/2017</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>01/10/2017</t>
+          <t>31/10/2017</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1508,7 +1508,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>01/10/2017</t>
+          <t>31/10/2017</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1531,7 +1531,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>01/10/2017</t>
+          <t>31/10/2017</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>01/10/2017</t>
+          <t>31/10/2017</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>01/10/2018</t>
+          <t>31/10/2018</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>01/10/2018</t>
+          <t>31/10/2018</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1623,7 +1623,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>01/10/2018</t>
+          <t>31/10/2018</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>01/10/2018</t>
+          <t>31/10/2018</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1669,7 +1669,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>01/10/2018</t>
+          <t>31/10/2018</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>01/10/2018</t>
+          <t>31/10/2018</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1715,7 +1715,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>01/10/2018</t>
+          <t>31/10/2018</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>01/10/2018</t>
+          <t>31/10/2018</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
+          <t>31/10/2019</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
+          <t>31/10/2019</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
+          <t>31/10/2019</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
+          <t>31/10/2019</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1853,7 +1853,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
+          <t>31/10/2019</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
+          <t>31/10/2019</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
+          <t>31/10/2019</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1922,7 +1922,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>01/10/2019</t>
+          <t>31/10/2019</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1945,7 +1945,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
+          <t>31/10/2020</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
+          <t>31/10/2020</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
+          <t>31/10/2020</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
+          <t>31/10/2020</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2037,7 +2037,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
+          <t>31/10/2020</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
+          <t>31/10/2020</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
+          <t>31/10/2020</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>01/10/2020</t>
+          <t>31/10/2020</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
+          <t>31/10/2021</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -2152,7 +2152,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
+          <t>31/10/2021</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
+          <t>31/10/2021</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
+          <t>31/10/2021</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
+          <t>31/10/2021</t>
         </is>
       </c>
       <c r="D78" t="n">
@@ -2244,7 +2244,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
+          <t>31/10/2021</t>
         </is>
       </c>
       <c r="D79" t="n">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
+          <t>31/10/2021</t>
         </is>
       </c>
       <c r="D80" t="n">
@@ -2290,7 +2290,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>01/10/2021</t>
+          <t>31/10/2021</t>
         </is>
       </c>
       <c r="D81" t="n">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
+          <t>31/10/2022</t>
         </is>
       </c>
       <c r="D82" t="n">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
+          <t>31/10/2022</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
+          <t>31/10/2022</t>
         </is>
       </c>
       <c r="D84" t="n">
@@ -2382,7 +2382,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
+          <t>31/10/2022</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -2405,7 +2405,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
+          <t>31/10/2022</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
+          <t>31/10/2022</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -2451,7 +2451,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
+          <t>31/10/2022</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>01/10/2022</t>
+          <t>31/10/2022</t>
         </is>
       </c>
       <c r="D89" t="n">
@@ -2497,7 +2497,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -2520,7 +2520,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -2543,7 +2543,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="D92" t="n">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="D93" t="n">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="D94" t="n">
@@ -2612,7 +2612,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="D95" t="n">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="D96" t="n">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>01/10/2023</t>
+          <t>31/10/2023</t>
         </is>
       </c>
       <c r="D97" t="n">
@@ -2666,6 +2666,190 @@
       </c>
       <c r="E97" t="n">
         <v>21.3</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Agricultura, pecuária, produção florestal, pesca e aquicultura</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>116</v>
+      </c>
+      <c r="E98" t="n">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Indústria geral</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>82</v>
+      </c>
+      <c r="E99" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Construção</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>83</v>
+      </c>
+      <c r="E100" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Comércio, reparação de veículos automotores e motocicletas</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>200</v>
+      </c>
+      <c r="E101" t="n">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Transporte, armazenagem e correio</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>50</v>
+      </c>
+      <c r="E102" t="n">
+        <v>4.9</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Alojamento e alimentação</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>58</v>
+      </c>
+      <c r="E103" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Informação, comunicação e atividades financeiras, imobiliárias, profissionais e administrativas</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>102</v>
+      </c>
+      <c r="E104" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Administração pública, defesa, seguridade social, educação, saúde humana e serviços sociais</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>209</v>
+      </c>
+      <c r="E105" t="n">
+        <v>20.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>